<commit_message>
Update - verbindingen begrippenkader gecontroleerd
</commit_message>
<xml_diff>
--- a/werkomgeving/voorbeeldmodel/begrippenkader/Fietsenwinkel.xlsx
+++ b/werkomgeving/voorbeeldmodel/begrippenkader/Fietsenwinkel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcobrattinga/GITREPO/mim-metamodel/werkomgeving/voorbeeldmodel/begrippenkader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28264E9D-192D-3049-810D-E68D414DFD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D75A474-0345-5F4D-BDEE-CF45AB53AC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="1920" windowWidth="31240" windowHeight="14520" activeTab="1" xr2:uid="{845DB935-A232-42CF-AB27-2E49A56C7476}"/>
+    <workbookView xWindow="3320" yWindow="1920" windowWidth="31240" windowHeight="14520" activeTab="2" xr2:uid="{845DB935-A232-42CF-AB27-2E49A56C7476}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemeen" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Relatietypen" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Begrippen!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Begrippen!$A$1:$J$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Kennisbronnen!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Relaties!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Termvormen!$A$1:$C$1</definedName>
@@ -91,7 +91,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">Een zo precies mogelijke verwijzing naar het deel van de kennisbron(nen) waaruit de betekenis van dit begrip is gehaald. Scheid meerdere kennisbronnen met een “;” en gebruik altijd de citeertitel uit het tabblad “Kennisbronnen” om de verwijzing te maken naar de gebruikte kennisbron, bijvoorbeeld: “Artikel 1:3 Awb”
 </t>
@@ -182,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="161">
   <si>
     <t>Naam model</t>
   </si>
@@ -298,30 +297,12 @@
     <t>leveringsdatum</t>
   </si>
   <si>
-    <t>volgnummer</t>
-  </si>
-  <si>
-    <t>versnellingen</t>
-  </si>
-  <si>
     <t>verkoopprijs</t>
   </si>
   <si>
-    <t>DFe verkoopprijs van de fiets, met twee decimalen, in Euro.</t>
-  </si>
-  <si>
-    <t>het volgummer van de fiets in één levering</t>
-  </si>
-  <si>
-    <t>het type aandrijving van de fiets</t>
-  </si>
-  <si>
     <t>de omvang van de fiets in dimensies vanaf voor tot achterband (opgepompt), uitersten van trappers of bak of bagagedrager, en hoogste punt vanaf de weg (stuur, zadel).</t>
   </si>
   <si>
-    <t>het aantal versnellingen van de fiets.</t>
-  </si>
-  <si>
     <t>Rubriek</t>
   </si>
   <si>
@@ -437,15 +418,6 @@
   </si>
   <si>
     <t>een [locatie] waar [fietsen] worden verkocht</t>
-  </si>
-  <si>
-    <t>een fysieke plek op aarde met een adres</t>
-  </si>
-  <si>
-    <t>Een adres is in beginsel een straatnaam, huisnummer en plaats, maar zou ook een geometrische aanduiding kunnen zijn.</t>
-  </si>
-  <si>
-    <t>Voor dit begrippenkader is niet van belang wat een adres zou kunnen zijn, maar vooral dat zo'n locatie te vinden in en een fysieke plek is.</t>
   </si>
   <si>
     <t>een fiets is een voertuig met twee of meer wielen dat door middel van menselijke kracht wordt voortbewogen</t>
@@ -579,6 +551,120 @@
   </si>
   <si>
     <t>goed</t>
+  </si>
+  <si>
+    <t>fietsenwinkelonderneming</t>
+  </si>
+  <si>
+    <t>Een fietsenwinkelonderneming is een [onderneming] die [fietsen] verkoopt in een [fietsenwinkel]</t>
+  </si>
+  <si>
+    <t>een fysieke plek op aarde met een [adres]</t>
+  </si>
+  <si>
+    <t>adres</t>
+  </si>
+  <si>
+    <t>Een adres is een administratieve aanduiding van een plek op aarde, bestaande uit de plaatsnaam, straatnaam en nummeraanduiding</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Fietsenwinkels maken gebruiken van adresbestanden, gebaseerd op openbare bronnen. Echter, mocht een opgegeven adres niet in deze bronnen voorkomen, dan wordt het wel als een adres gezien. In zo'n geval zal een dergelijk adres ook geen postcode hebben.</t>
+  </si>
+  <si>
+    <t>Adres volgt uit de afspraken die fietsenwinkels met elkaar hebben gemaakt en wijkt deels af van de definitie uit de openbare bronnen (zoals bijvoorbeeld de Basisregistratie adressen en gebouwen)</t>
+  </si>
+  <si>
+    <t>Een postcode is een unieke combinatie van cijfers en letters voor een groep van één of meer [adressen]</t>
+  </si>
+  <si>
+    <t>bekend adres</t>
+  </si>
+  <si>
+    <t>onbekend adres</t>
+  </si>
+  <si>
+    <t>Een onbekend adres ie een [adres] dat niet voorkomt in openbare bronnen</t>
+  </si>
+  <si>
+    <t>Een bekend adres is een [adres] dat voorkomt in openbare bronnen</t>
+  </si>
+  <si>
+    <t>adressen</t>
+  </si>
+  <si>
+    <t>postadres</t>
+  </si>
+  <si>
+    <t>Een postadres is een [adres] waar post naartoe gestuurd kan worden</t>
+  </si>
+  <si>
+    <t>Het postadres wordt onder meer gebruikt voor het versturen van fakturen en aanbiedingen naar klanten. Een postadres is een locatie, maar hoeft niet de locatie te zijn waar de klant zijn fiets geleverd wenst te hebben</t>
+  </si>
+  <si>
+    <t>leveringsadres</t>
+  </si>
+  <si>
+    <t>faktuuradres</t>
+  </si>
+  <si>
+    <t>Een faktuuradres is een [postadres] waar formele post naartoe gestuurd wordt</t>
+  </si>
+  <si>
+    <t>Onder formele post vallen in ieder geval faktoren, maar ook aanmaningen en andere verplichting-gerelateerde post. Afgesproken is dat formele post altijd naar een bekend adres wordt gestuurd.</t>
+  </si>
+  <si>
+    <t>Een leveringsadres is een [adres] van een [locatie] waar een [levering] wordt afgeleverd</t>
+  </si>
+  <si>
+    <t>is uniek nummer van</t>
+  </si>
+  <si>
+    <t>een aandrijving is een constructie op een [fiets] waarmee de spierkracht wordt overgebracht op de wielen</t>
+  </si>
+  <si>
+    <t>riemaandrijving</t>
+  </si>
+  <si>
+    <t>kettingaandrijving</t>
+  </si>
+  <si>
+    <t>Een riemaandrijving is een aandrijving met behulp van een riem</t>
+  </si>
+  <si>
+    <t>Een kettingaandrijving is een aandrijving met behulp van een ketting</t>
+  </si>
+  <si>
+    <t>Een kettingaandrijving is de meest gebruikte vorm van aandrijving op een fiets. Een fiets met een derrailleur (zoals de meeste racefietsen, mountainbikes en tourfietsen) vereist een kettingaandrijving.</t>
+  </si>
+  <si>
+    <t>Bij een riemaandrijving is de ketting vervangen door een riem. De riem heeft minder onderhoud nodig en is ook stiller. Het is echter niet mogelijk om een riem te gebruiken met een derrailleur, een naafversnelling is noodzakelijk.</t>
+  </si>
+  <si>
+    <t>fietsversnelling</t>
+  </si>
+  <si>
+    <t>Een fietsversnelling is een constructie op een [fiets] waarmee de verhouding tussen de [aandrijving] en de wielen geregeld kan worden</t>
+  </si>
+  <si>
+    <t>naafversnelling</t>
+  </si>
+  <si>
+    <t>Een naafversnelling is een [fietsversnelling] die in een gesloten constructie in de naaf van een wiel is verwerkt</t>
+  </si>
+  <si>
+    <t>derailleurversnelling</t>
+  </si>
+  <si>
+    <t>Een derailleurversnelling is een [fietsversnelling] die in een open constructie in samenhang met de [kettingaandrijving] is geconstrueerd</t>
+  </si>
+  <si>
+    <t>Een bedrag in euro's inclusief BTW waarvoor een [artikel] gekocht mag worden</t>
+  </si>
+  <si>
+    <t>De verkoopprijs is het bedrag dat de koper van een artikel daadwerkelijk betaald voor het artikel</t>
   </si>
 </sst>
 </file>
@@ -1432,10 +1518,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1443,15 +1529,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1459,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1467,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1491,7 +1577,7 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="str">
         <f ca="1">UPPER(_xlfn.CONCAT(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>96ABC001-0B35-45A6-875D-13216435BBC5</v>
+        <v>E1D97832-7E74-4B1A-A610-9AAA73EAACFA</v>
       </c>
       <c r="B9" s="35"/>
     </row>
@@ -1542,13 +1628,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E3E14F-D85B-4917-B2C0-1103088DAC01}">
   <sheetPr codeName="Blad2"/>
-  <dimension ref="A1:J404"/>
+  <dimension ref="A1:J403"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1571,7 +1657,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>5</v>
@@ -1603,17 +1689,17 @@
         <v>23</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -1625,7 +1711,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>29</v>
@@ -1633,7 +1719,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="25"/>
       <c r="F3" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -1645,7 +1731,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>31</v>
@@ -1663,10 +1749,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="25"/>
@@ -1681,10 +1767,10 @@
         <v>25</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>33</v>
@@ -1698,13 +1784,13 @@
     </row>
     <row r="7" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D7" s="33" t="s">
         <v>34</v>
@@ -1718,13 +1804,13 @@
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="25"/>
@@ -1734,24 +1820,20 @@
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>86</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D9" s="33"/>
       <c r="E9" s="25"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="11" t="s">
-        <v>87</v>
-      </c>
+      <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
@@ -1761,17 +1843,17 @@
         <v>26</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="11" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -1780,17 +1862,17 @@
     </row>
     <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="25" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -1800,16 +1882,16 @@
     </row>
     <row r="12" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="11"/>
@@ -1823,10 +1905,10 @@
         <v>36</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="25"/>
@@ -1841,10 +1923,10 @@
         <v>37</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="25"/>
@@ -1856,16 +1938,16 @@
     </row>
     <row r="15" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="11"/>
@@ -1874,15 +1956,15 @@
       <c r="I15" s="11"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="25"/>
@@ -1892,15 +1974,15 @@
       <c r="I16" s="11"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="25"/>
@@ -1910,15 +1992,15 @@
       <c r="I17" s="11"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="25"/>
@@ -1928,17 +2010,19 @@
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="11"/>
+        <v>159</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>160</v>
+      </c>
       <c r="E19" s="25"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -1948,100 +2032,120 @@
     </row>
     <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>41</v>
+        <v>91</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="D20" s="11"/>
-      <c r="E20" s="25"/>
+      <c r="E20" s="25" t="s">
+        <v>122</v>
+      </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B22" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="11"/>
       <c r="E22" s="25"/>
       <c r="F22" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" s="11" t="s">
         <v>114</v>
       </c>
+      <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>122</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D23" s="11"/>
       <c r="E23" s="25"/>
-      <c r="F23" s="11" t="s">
-        <v>123</v>
-      </c>
+      <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+    <row r="24" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>129</v>
+      </c>
       <c r="E24" s="25"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
+      <c r="F24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>130</v>
+      </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="12"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="C25" s="11"/>
+    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>131</v>
+      </c>
       <c r="D25" s="11"/>
       <c r="E25" s="25"/>
       <c r="F25" s="11"/>
@@ -2050,9 +2154,16 @@
       <c r="I25" s="11"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="C26" s="11"/>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>135</v>
+      </c>
       <c r="D26" s="11"/>
       <c r="E26" s="25"/>
       <c r="F26" s="11"/>
@@ -2061,9 +2172,16 @@
       <c r="I26" s="11"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="C27" s="11"/>
+    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="D27" s="11"/>
       <c r="E27" s="25"/>
       <c r="F27" s="11"/>
@@ -2072,10 +2190,19 @@
       <c r="I27" s="11"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+    <row r="28" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>139</v>
+      </c>
       <c r="E28" s="25"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -2083,9 +2210,16 @@
       <c r="I28" s="11"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="C29" s="11"/>
+    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="D29" s="11"/>
       <c r="E29" s="25"/>
       <c r="F29" s="11"/>
@@ -2094,10 +2228,19 @@
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+    <row r="30" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>143</v>
+      </c>
       <c r="E30" s="25"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -2105,10 +2248,19 @@
       <c r="I30" s="11"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+    <row r="31" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>152</v>
+      </c>
       <c r="E31" s="25"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -2116,10 +2268,19 @@
       <c r="I31" s="11"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
+    <row r="32" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>151</v>
+      </c>
       <c r="E32" s="25"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -2127,9 +2288,16 @@
       <c r="I32" s="11"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="C33" s="11"/>
+    <row r="33" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>156</v>
+      </c>
       <c r="D33" s="11"/>
       <c r="E33" s="25"/>
       <c r="F33" s="11"/>
@@ -2138,9 +2306,16 @@
       <c r="I33" s="11"/>
       <c r="J33" s="12"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="C34" s="11"/>
+    <row r="34" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="D34" s="11"/>
       <c r="E34" s="25"/>
       <c r="F34" s="11"/>
@@ -6198,29 +6373,18 @@
       <c r="J402" s="12"/>
     </row>
     <row r="403" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A403" s="8"/>
-      <c r="C403" s="11"/>
-      <c r="D403" s="11"/>
-      <c r="E403" s="25"/>
-      <c r="F403" s="11"/>
-      <c r="G403" s="11"/>
-      <c r="H403" s="11"/>
-      <c r="I403" s="11"/>
-      <c r="J403" s="12"/>
-    </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A404" s="13"/>
-      <c r="C404" s="14"/>
-      <c r="D404" s="14"/>
-      <c r="E404" s="26"/>
-      <c r="F404" s="14"/>
-      <c r="G404" s="14"/>
-      <c r="H404" s="14"/>
-      <c r="I404" s="14"/>
-      <c r="J404" s="15"/>
+      <c r="A403" s="13"/>
+      <c r="C403" s="14"/>
+      <c r="D403" s="14"/>
+      <c r="E403" s="26"/>
+      <c r="F403" s="14"/>
+      <c r="G403" s="14"/>
+      <c r="H403" s="14"/>
+      <c r="I403" s="14"/>
+      <c r="J403" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J21" xr:uid="{F2E3E14F-D85B-4917-B2C0-1103088DAC01}"/>
+  <autoFilter ref="A1:J20" xr:uid="{F2E3E14F-D85B-4917-B2C0-1103088DAC01}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;L_x000D_&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022B C2 - Restricted use </oddFooter>
@@ -6233,8 +6397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32BF457-35B9-EC4C-8B52-40D543FFA94A}">
   <dimension ref="A1:E398"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6248,16 +6412,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -6268,13 +6432,13 @@
         <v>37</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E2" s="18"/>
     </row>
@@ -6283,13 +6447,13 @@
         <v>26</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E3" s="18"/>
     </row>
@@ -6298,13 +6462,13 @@
         <v>23</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E4" s="18"/>
     </row>
@@ -6313,43 +6477,43 @@
         <v>25</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E7" s="18"/>
     </row>
@@ -6358,132 +6522,242 @@
         <v>24</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E8" s="18"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E16" s="18"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E17" s="18"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E18" s="18"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>72</v>
+      </c>
       <c r="E19" s="18"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -8335,9 +8609,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{485D0114-7B97-EC49-91AB-A82ED160F552}">
           <x14:formula1>
-            <xm:f>Begrippen!$A$2:$A$10033</xm:f>
+            <xm:f>Begrippen!$A$2:$A$10032</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576 A2:A1048576</xm:sqref>
+          <xm:sqref>A2:A1048576 C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8351,7 +8625,7 @@
   <dimension ref="A1:C400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8373,16 +8647,20 @@
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>136</v>
+      </c>
       <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -10420,81 +10698,81 @@
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -13677,72 +13955,72 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
omvang uit het model gehaald
</commit_message>
<xml_diff>
--- a/werkomgeving/voorbeeldmodel/begrippenkader/Fietsenwinkel.xlsx
+++ b/werkomgeving/voorbeeldmodel/begrippenkader/Fietsenwinkel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcobrattinga/GITREPO/mim-metamodel/werkomgeving/voorbeeldmodel/begrippenkader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775848ED-D046-B14A-AD2C-E1123FD5F1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882A906F-774F-2443-821D-C8881F3A7984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3320" yWindow="1920" windowWidth="31240" windowHeight="14520" activeTab="1" xr2:uid="{845DB935-A232-42CF-AB27-2E49A56C7476}"/>
   </bookViews>
@@ -21,9 +21,9 @@
     <sheet name="Relatietypen" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Begrippen!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Begrippen!$A$1:$J$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Kennisbronnen!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Relaties!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Relaties!$A$1:$E$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Termvormen!$A$1:$C$1</definedName>
     <definedName name="Code_kennisgebied">#REF!</definedName>
     <definedName name="Kennisgebied">#REF!</definedName>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="198">
   <si>
     <t>Naam model</t>
   </si>
@@ -273,9 +273,6 @@
     <t>garantienummer</t>
   </si>
   <si>
-    <t>omvang</t>
-  </si>
-  <si>
     <t>Een sportfiets heeft over het algemeen geen licht of spatborden, en is zo licht als mogelijk uitgevoerd. Voorbeeld: Racefiets, mountainbike</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
   </si>
   <si>
     <t>verkoopprijs</t>
-  </si>
-  <si>
-    <t>de omvang van de fiets in dimensies vanaf voor tot achterband (opgepompt), uitersten van trappers of bak of bagagedrager, en hoogste punt vanaf de weg (stuur, zadel).</t>
   </si>
   <si>
     <t>Rubriek</t>
@@ -526,9 +520,6 @@
     <t>Verkoop</t>
   </si>
   <si>
-    <t>De omvang van een [artikel] in hoogte, breedte en lengte</t>
-  </si>
-  <si>
     <t>goed</t>
   </si>
   <si>
@@ -538,9 +529,6 @@
     <t>Een fietsenwinkelonderneming is een [onderneming] die [fietsen] verkoopt in een [fietsenwinkel]</t>
   </si>
   <si>
-    <t>een fysieke plek op aarde met een [adres]</t>
-  </si>
-  <si>
     <t>adres</t>
   </si>
   <si>
@@ -646,15 +634,9 @@
     <t>De verkoopprijs is het bedrag dat de koper van een artikel daadwerkelijk betaald voor het artikel</t>
   </si>
   <si>
-    <t>De datum van de [levering] van één of meerdere artikelen</t>
-  </si>
-  <si>
     <t>leverancier</t>
   </si>
   <si>
-    <t>Een gebeurtenis waarbij [artikelen] op een afgesproken [locatie] worden gebracht op basis van een eerder afgesproken overeenkomst</t>
-  </si>
-  <si>
     <t>ondernemingen</t>
   </si>
   <si>
@@ -712,9 +694,6 @@
     <t>leveranciers</t>
   </si>
   <si>
-    <t>De naam van een [onderneming] zoals deze door de onderneming in de praktijk wordt gebruikt</t>
-  </si>
-  <si>
     <t>De handelsnaam staat bijvoorbeeld op de gevel van locatie waar goederen worden verkocht en wordt gebruikt in communicatie met klanten en leveranciers</t>
   </si>
   <si>
@@ -785,6 +764,18 @@
   </si>
   <si>
     <t>De framemaat wordt in centimeters gemeten vanaf het hart van de trapas tot aan het punt waar het zadel uit het frame (zou) komen</t>
+  </si>
+  <si>
+    <t>Een handelsnaam is de naam van een [onderneming] zoals deze door de onderneming in de praktijk wordt gebruikt</t>
+  </si>
+  <si>
+    <t>een locatie is een fysieke plek op aarde met een [adres]</t>
+  </si>
+  <si>
+    <t>Een leveringsdatum is de datum van de [levering] van één of meerdere artikelen</t>
+  </si>
+  <si>
+    <t>Een levering is een gebeurtenis waarbij [artikelen] op een afgesproken [locatie] worden gebracht op basis van een eerder afgesproken overeenkomst</t>
   </si>
 </sst>
 </file>
@@ -1638,10 +1629,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1649,15 +1640,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1665,7 +1656,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1673,7 +1664,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1697,7 +1688,7 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="str">
         <f ca="1">UPPER(_xlfn.CONCAT(DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4),"-","4",DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(8,11)),DEC2HEX(RANDBETWEEN(0,POWER(16,3)),3),"-",DEC2HEX(RANDBETWEEN(0,POWER(16,8)),8),DEC2HEX(RANDBETWEEN(0,POWER(16,4)),4)))</f>
-        <v>DED71C99-F4E5-44F0-9800-FFB22A7F1148</v>
+        <v>CCD5E3B7-35B6-420E-BEAD-9EA47A0FAB7A</v>
       </c>
       <c r="B9" s="35"/>
     </row>
@@ -1748,13 +1739,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E3E14F-D85B-4917-B2C0-1103088DAC01}">
   <sheetPr codeName="Blad2"/>
-  <dimension ref="A1:J404"/>
+  <dimension ref="A1:J402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1777,7 +1768,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>5</v>
@@ -1809,17 +1800,17 @@
         <v>23</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -1831,17 +1822,17 @@
         <v>24</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -1853,10 +1844,10 @@
         <v>29</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="25"/>
@@ -1866,33 +1857,35 @@
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="11"/>
       <c r="E5" s="25"/>
-      <c r="F5" s="18"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>90</v>
+        <v>167</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>31</v>
@@ -1904,18 +1897,18 @@
       <c r="I6" s="11"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>32</v>
+        <v>170</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="11"/>
@@ -1924,19 +1917,17 @@
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>177</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="D8" s="33"/>
       <c r="E8" s="25"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -1944,98 +1935,100 @@
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="33"/>
+        <v>72</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="E9" s="25"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>26</v>
+        <v>188</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>74</v>
+        <v>189</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>75</v>
+        <v>193</v>
       </c>
       <c r="E10" s="25"/>
-      <c r="F10" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>195</v>
+        <v>85</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="E11" s="25"/>
+        <v>80</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="25" t="s">
+        <v>79</v>
+      </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C12" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="25" t="s">
-        <v>81</v>
-      </c>
+      <c r="E12" s="25"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>83</v>
+        <v>186</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="11"/>
@@ -2044,19 +2037,17 @@
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>194</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="D14" s="11"/>
       <c r="E14" s="25"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -2064,17 +2055,19 @@
       <c r="I14" s="11"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="D15" s="11"/>
+        <v>197</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="E15" s="25"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -2082,19 +2075,17 @@
       <c r="I15" s="11"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>66</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D16" s="11"/>
       <c r="E16" s="25"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
@@ -2104,13 +2095,13 @@
     </row>
     <row r="17" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="25"/>
@@ -2120,17 +2111,19 @@
       <c r="I17" s="11"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="11"/>
+        <v>148</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>149</v>
+      </c>
       <c r="E18" s="25"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -2138,117 +2131,121 @@
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>147</v>
+        <v>84</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="D19" s="11"/>
-      <c r="E19" s="25"/>
+      <c r="E19" s="25" t="s">
+        <v>112</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>153</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="11"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="F20" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="11"/>
+        <v>104</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>97</v>
-      </c>
       <c r="C22" s="11" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="25"/>
-      <c r="F22" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>99</v>
-      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G23" s="11"/>
+        <v>60</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>119</v>
+      </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="25"/>
@@ -2258,39 +2255,33 @@
       <c r="I24" s="11"/>
       <c r="J24" s="12"/>
     </row>
-    <row r="25" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>122</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D25" s="11"/>
       <c r="E25" s="25"/>
-      <c r="F25" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>123</v>
-      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="25"/>
@@ -2300,17 +2291,19 @@
       <c r="I26" s="11"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C27" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="11"/>
       <c r="E27" s="25"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -2320,13 +2313,13 @@
     </row>
     <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="25"/>
@@ -2341,7 +2334,7 @@
         <v>130</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>131</v>
@@ -2356,17 +2349,19 @@
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D30" s="11"/>
+        <v>138</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>141</v>
+      </c>
       <c r="E30" s="25"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -2376,16 +2371,16 @@
     </row>
     <row r="31" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="11"/>
@@ -2394,19 +2389,17 @@
       <c r="I31" s="11"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" s="11" t="s">
         <v>145</v>
       </c>
+      <c r="D32" s="11"/>
       <c r="E32" s="25"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -2414,19 +2407,17 @@
       <c r="I32" s="11"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>144</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="D33" s="11"/>
       <c r="E33" s="25"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -2436,13 +2427,13 @@
     </row>
     <row r="34" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="25"/>
@@ -2452,33 +2443,39 @@
       <c r="I34" s="11"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D35" s="11"/>
+        <v>155</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>156</v>
+      </c>
       <c r="E35" s="25"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+      <c r="F35" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>157</v>
+      </c>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="25"/>
@@ -2488,44 +2485,40 @@
       <c r="I36" s="11"/>
       <c r="J36" s="12"/>
     </row>
-    <row r="37" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>162</v>
-      </c>
+      <c r="D37" s="11"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>163</v>
-      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="12"/>
     </row>
-    <row r="38" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="25"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
+      <c r="G38" s="11" t="s">
+        <v>163</v>
+      </c>
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
       <c r="J38" s="12"/>
@@ -2535,10 +2528,10 @@
         <v>164</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="25"/>
@@ -2548,36 +2541,20 @@
       <c r="I39" s="11"/>
       <c r="J39" s="12"/>
     </row>
-    <row r="40" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>168</v>
-      </c>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="25"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="11" t="s">
-        <v>169</v>
-      </c>
+      <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="12"/>
     </row>
-    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>171</v>
-      </c>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="25"/>
       <c r="F41" s="11"/>
@@ -6547,40 +6524,18 @@
       <c r="J401" s="12"/>
     </row>
     <row r="402" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A402" s="8"/>
-      <c r="C402" s="11"/>
-      <c r="D402" s="11"/>
-      <c r="E402" s="25"/>
-      <c r="F402" s="11"/>
-      <c r="G402" s="11"/>
-      <c r="H402" s="11"/>
-      <c r="I402" s="11"/>
-      <c r="J402" s="12"/>
-    </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A403" s="8"/>
-      <c r="C403" s="11"/>
-      <c r="D403" s="11"/>
-      <c r="E403" s="25"/>
-      <c r="F403" s="11"/>
-      <c r="G403" s="11"/>
-      <c r="H403" s="11"/>
-      <c r="I403" s="11"/>
-      <c r="J403" s="12"/>
-    </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A404" s="13"/>
-      <c r="C404" s="14"/>
-      <c r="D404" s="14"/>
-      <c r="E404" s="26"/>
-      <c r="F404" s="14"/>
-      <c r="G404" s="14"/>
-      <c r="H404" s="14"/>
-      <c r="I404" s="14"/>
-      <c r="J404" s="15"/>
+      <c r="A402" s="13"/>
+      <c r="C402" s="14"/>
+      <c r="D402" s="14"/>
+      <c r="E402" s="26"/>
+      <c r="F402" s="14"/>
+      <c r="G402" s="14"/>
+      <c r="H402" s="14"/>
+      <c r="I402" s="14"/>
+      <c r="J402" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J21" xr:uid="{F2E3E14F-D85B-4917-B2C0-1103088DAC01}"/>
+  <autoFilter ref="A1:J19" xr:uid="{F2E3E14F-D85B-4917-B2C0-1103088DAC01}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;L_x000D_&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022B C2 - Restricted use </oddFooter>
@@ -6593,9 +6548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32BF457-35B9-EC4C-8B52-40D543FFA94A}">
   <dimension ref="A1:E398"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6608,16 +6561,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -6625,16 +6578,16 @@
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" s="18"/>
     </row>
@@ -6643,13 +6596,13 @@
         <v>26</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" s="18"/>
     </row>
@@ -6658,13 +6611,13 @@
         <v>23</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="18"/>
     </row>
@@ -6673,43 +6626,43 @@
         <v>25</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E7" s="18"/>
     </row>
@@ -6718,463 +6671,463 @@
         <v>24</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E28" s="18"/>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E29" s="18"/>
     </row>
     <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E34" s="18"/>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E37" s="18"/>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E38" s="18"/>
     </row>
@@ -7183,28 +7136,28 @@
         <v>27</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E40" s="18"/>
     </row>
@@ -7213,58 +7166,58 @@
         <v>29</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E42" s="18"/>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E44" s="18"/>
     </row>
@@ -9039,6 +8992,7 @@
       <c r="E398" s="20"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E44" xr:uid="{A32BF457-35B9-EC4C-8B52-40D543FFA94A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
@@ -9047,17 +9001,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{485D0114-7B97-EC49-91AB-A82ED160F552}">
-          <x14:formula1>
-            <xm:f>Begrippen!$A$2:$A$10033</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A1048576 C2:C1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F1C7FFFB-56CB-5943-BF4A-732290B82ED6}">
           <x14:formula1>
             <xm:f>Relatietypen!$A$2:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{485D0114-7B97-EC49-91AB-A82ED160F552}">
+          <x14:formula1>
+            <xm:f>Begrippen!$A$2:$A$10031</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A1048576 C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9093,55 +9047,55 @@
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>91</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>93</v>
       </c>
       <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C7" s="19"/>
     </row>
@@ -11160,81 +11114,81 @@
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -14417,83 +14371,83 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>